<commit_message>
dodano kilka wstepnie opracowanych taskow do kolejnego sprintu
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Damian\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\IPP30 Projects\SmartShop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pomysły" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="56">
   <si>
     <t>Story</t>
   </si>
@@ -192,6 +192,33 @@
   </si>
   <si>
     <t>Wklej specjalnie -&gt; Zachowaj szerokości kolumn źródłowych</t>
+  </si>
+  <si>
+    <t>Konto na smarterasp.net</t>
+  </si>
+  <si>
+    <t>prawidłowo utworzone konto na smarterasp.net</t>
+  </si>
+  <si>
+    <t>Mock aplikacji klienckiej</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć utworzone konto na smartertasp.net abym mógł hostować tam webservice.</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć zaprojektowany i utworzony mock aplikacji klienckiej abym mógł zaimplementować do niego logike i podpiąć usługi</t>
+  </si>
+  <si>
+    <t>Utworzenie webservicu</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć utworzony webservice abym móg komunikować się z nim z aplikacji klienckiej</t>
+  </si>
+  <si>
+    <t>Upload webservicu na smartertasp.net</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć wrzucony webservice na smarterasp.net abym mógł komunikować się z nim zdalnie z aplikacji klienckiej</t>
   </si>
 </sst>
 </file>
@@ -362,8 +389,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -371,1463 +404,17 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="178">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="34">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2173,8 +760,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="177"/>
-      <tableStyleElement type="headerRow" dxfId="176"/>
+      <tableStyleElement type="wholeTable" dxfId="33"/>
+      <tableStyleElement type="headerRow" dxfId="32"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -2453,7 +1040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -2474,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G11"/>
+  <dimension ref="B2:G15"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2491,32 +1078,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="14"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2678,6 +1265,41 @@
       </c>
       <c r="G11" s="7" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2962,39 +1584,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="2:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="14"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3135,7 +1757,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="11" t="s">
         <v>41</v>
       </c>
       <c r="E13" s="9">
@@ -3469,7 +2091,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="12" t="s">
         <v>45</v>
       </c>
       <c r="F8" s="1" t="s">

</xml_diff>

<commit_message>
uaktualniono backlog, dodano zdjecie schematu bazy danych
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pomysły" sheetId="2" r:id="rId1"/>
     <sheet name="Backlog" sheetId="5" r:id="rId2"/>
-    <sheet name="Sprint 1" sheetId="3" r:id="rId3"/>
-    <sheet name="Słowniki" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint 2" sheetId="6" r:id="rId3"/>
+    <sheet name="Sprint 1" sheetId="3" r:id="rId4"/>
+    <sheet name="Słowniki" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="88">
   <si>
     <t>Story</t>
   </si>
@@ -134,9 +135,6 @@
   </si>
   <si>
     <t>Niezrealizowane</t>
-  </si>
-  <si>
-    <t>#2</t>
   </si>
   <si>
     <t>#3</t>
@@ -197,18 +195,9 @@
     <t>Konto na smarterasp.net</t>
   </si>
   <si>
-    <t>prawidłowo utworzone konto na smarterasp.net</t>
-  </si>
-  <si>
-    <t>Mock aplikacji klienckiej</t>
-  </si>
-  <si>
     <t>Jako developer chcę mieć utworzone konto na smartertasp.net abym mógł hostować tam webservice.</t>
   </si>
   <si>
-    <t>Jako developer chcę mieć zaprojektowany i utworzony mock aplikacji klienckiej abym mógł zaimplementować do niego logike i podpiąć usługi</t>
-  </si>
-  <si>
     <t>Utworzenie webservicu</t>
   </si>
   <si>
@@ -219,13 +208,160 @@
   </si>
   <si>
     <t>Jako developer chcę mieć wrzucony webservice na smarterasp.net abym mógł komunikować się z nim zdalnie z aplikacji klienckiej</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć zaprojektowany i utworzony mock głównego widoku aplikacji klienckiej abym mógł zaimplementować do niego logike i podpiąć usługi</t>
+  </si>
+  <si>
+    <t>#2   06.04 - 27.04</t>
+  </si>
+  <si>
+    <t>Mock głównego widoku aplikacji klienckiej</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć utworzone modele danych odpowiadające tabelą w bazie danych, abym mógł korzystać z nich w aplikacji</t>
+  </si>
+  <si>
+    <t>klasy modeli dla tabel z bazy danych w projekcie SmartShopWpf, projekt się kompiluje</t>
+  </si>
+  <si>
+    <t>prawidłowo utworzone konto na smarterasp.net, przekazanie członkom zespołu informacji o danych do logowania</t>
+  </si>
+  <si>
+    <t>możliwość wykonania metod HTTP dla każdej z tabeli i uzyskanie prawidłowej odpowiedzi, projekt się kompiluje</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> prawidłowo zuploadowany webservice na smarterasp.net, możliwość wykonania metod HTTP dla każdej z tabeli i uzyskanie prawidłowej odpowiedzi</t>
+  </si>
+  <si>
+    <t>mock który jest dopasowany graficznie (kolory, czcionki itp) do mocka widoku logowania, podoba się wszystkim! i jest przygotowany do implementacji logiki zawartej w specyfikacji. Projekt się kompiluje.</t>
+  </si>
+  <si>
+    <t>Modele danych WPF</t>
+  </si>
+  <si>
+    <t>Zabezpieczenie brancha develop</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć zmodyfikowane ustawienia brancha develop, aby konieczne było wykonanie review przed commitem/mergem</t>
+  </si>
+  <si>
+    <t>zablokowana możliwość commitowania/mergowania do brancha develop, bez wcześniejszego wykonania rewiew</t>
+  </si>
+  <si>
+    <t>Mock widoku logowania</t>
+  </si>
+  <si>
+    <t>Jako developer chce mieć zaprojektowany i utworzony mock widoku logowania do aplikacji, abym mógł podpiąć do niego logikę i usługi weryfikujące poprawność wpisywanych danych logujących do systemu</t>
+  </si>
+  <si>
+    <t>mock który jest dopasowany graficznie (kolory, czcionki itp) do mocka widoku głównego, podoba się wszystkim! i jest przygotowany do implementacji logiki logowania. Projekt się kompiluje.</t>
+  </si>
+  <si>
+    <t>Modele danych WebApp</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć utworzone modele danych odpowiadające tabelą w bazie danych, abym mógł korzystać z nich w kontrolerach</t>
+  </si>
+  <si>
+    <t>klasy modeli dla tabel z bazy danych w projekcie SmartShopWebApp, projekt się kompiluje</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć zmodyfikowaną bazę danych, abym mógł przechowywać w niej informacje na temat kategorii danego produktu</t>
+  </si>
+  <si>
+    <t>Kategoria produktu w bazie danych</t>
+  </si>
+  <si>
+    <t>możliwość przechowywania informacji o kategorii produktu w bazie danych</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć zmodyfikowaną bazę danych, abym mógł przechowywać w niej zdjęcie danego produktu</t>
+  </si>
+  <si>
+    <t>pole w bazie danych przechowujące zdjęcie produktu</t>
+  </si>
+  <si>
+    <t>Zdjęcie produktu w bazie danych</t>
+  </si>
+  <si>
+    <t>Przykładowe produkty w bazie danych</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć dodane przykładowe produkty do bazy danych abym mógł je wykorzystywać w aplikacji</t>
+  </si>
+  <si>
+    <t>co najmniej 100 produktów w bazie danych z uzupełnionymi wszystkimi polami</t>
+  </si>
+  <si>
+    <t>Przygotowanie zdjęć produktów</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć przygotowane zdjęcia dla produktów abym mógł je dodać do rekordów w bazie danych i wyświetlać je w aplikacji klienckiej</t>
+  </si>
+  <si>
+    <t>minimum 100 zdjęć, stosunkowo małych, o jednakowych wymiarach</t>
+  </si>
+  <si>
+    <t>Przejście pomiędzy widokami</t>
+  </si>
+  <si>
+    <t>Jako developer chce mieć zaimplementowane połączenie pomiędzy widokami logowania i głównym tak aby po zalogowaniu uruchamiał się widok główny aplikacji</t>
+  </si>
+  <si>
+    <t>przejście do widoku głównego, po naciśnięciu odpowiedniego przycisku w widoku logowania, przekazania danych o zalogowanym użytkowniku pomiędzy widokami</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Czas realizacji: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>06.04 - 27.04</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Suma </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>SP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>:</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,6 +456,13 @@
       <charset val="238"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -368,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -398,6 +541,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -410,11 +562,1060 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="138">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -760,8 +1961,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="33"/>
-      <tableStyleElement type="headerRow" dxfId="32"/>
+      <tableStyleElement type="wholeTable" dxfId="137"/>
+      <tableStyleElement type="headerRow" dxfId="136"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1051,7 +2252,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1061,10 +2262,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G15"/>
+  <dimension ref="B2:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,10 +2279,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -1124,7 +2325,7 @@
         <v>31</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -1144,7 +2345,7 @@
         <v>31</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -1164,7 +2365,7 @@
         <v>31</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="75" x14ac:dyDescent="0.25">
@@ -1184,7 +2385,7 @@
         <v>31</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -1204,7 +2405,7 @@
         <v>31</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -1224,7 +2425,7 @@
         <v>31</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -1244,7 +2445,7 @@
         <v>31</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -1264,54 +2465,283 @@
         <v>31</v>
       </c>
       <c r="G11" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="7">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="6" t="s">
+    <row r="13" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B13" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="7">
+        <v>5</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="D15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="7">
+        <v>1</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="G15" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>55</v>
       </c>
+      <c r="D16" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="13">
+        <v>3</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="7">
+        <v>1</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="7">
+        <v>3</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="7">
+        <v>1</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="7">
+        <v>3</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="7">
+        <v>5</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="7">
+        <v>1</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{35DA5DFD-158A-4A96-AFD3-16E6826D71F1}">
+          <x14:cfRule type="cellIs" priority="13" operator="equal" id="{35DA5DFD-158A-4A96-AFD3-16E6826D71F1}">
             <xm:f>Słowniki!$C$3</xm:f>
             <x14:dxf>
               <font>
@@ -1324,7 +2754,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{0EF4BF86-951E-4041-96BC-970E20B0F305}">
+          <x14:cfRule type="cellIs" priority="14" operator="equal" id="{0EF4BF86-951E-4041-96BC-970E20B0F305}">
             <xm:f>Słowniki!$C$2</xm:f>
             <x14:dxf>
               <font>
@@ -1337,10 +2767,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G11</xm:sqref>
+          <xm:sqref>G11 G13 G15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="15" operator="equal" id="{8CC48237-1EF7-42C0-8632-8CF6FA73EAAC}">
+          <x14:cfRule type="cellIs" priority="27" operator="equal" id="{8CC48237-1EF7-42C0-8632-8CF6FA73EAAC}">
             <xm:f>Słowniki!$C$3</xm:f>
             <x14:dxf>
               <font>
@@ -1353,7 +2783,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="16" operator="equal" id="{D4C76A03-45DE-4A75-9EB4-91E96096B768}">
+          <x14:cfRule type="cellIs" priority="28" operator="equal" id="{D4C76A03-45DE-4A75-9EB4-91E96096B768}">
             <xm:f>Słowniki!$C$2</xm:f>
             <x14:dxf>
               <font>
@@ -1369,7 +2799,7 @@
           <xm:sqref>G4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="13" operator="equal" id="{20C769E0-576E-4A5B-833F-BD175DCC8383}">
+          <x14:cfRule type="cellIs" priority="25" operator="equal" id="{20C769E0-576E-4A5B-833F-BD175DCC8383}">
             <xm:f>Słowniki!$C$3</xm:f>
             <x14:dxf>
               <font>
@@ -1382,7 +2812,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="14" operator="equal" id="{104971B7-D297-494A-AD75-9138BA5AC24C}">
+          <x14:cfRule type="cellIs" priority="26" operator="equal" id="{104971B7-D297-494A-AD75-9138BA5AC24C}">
             <xm:f>Słowniki!$C$2</xm:f>
             <x14:dxf>
               <font>
@@ -1398,7 +2828,7 @@
           <xm:sqref>G5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="11" operator="equal" id="{F781F71C-1B94-4299-AC7C-06FA0D1D02FD}">
+          <x14:cfRule type="cellIs" priority="23" operator="equal" id="{F781F71C-1B94-4299-AC7C-06FA0D1D02FD}">
             <xm:f>Słowniki!$C$3</xm:f>
             <x14:dxf>
               <font>
@@ -1411,7 +2841,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="12" operator="equal" id="{88C79D3D-BA54-4078-BD9E-2F9BC3DEFB72}">
+          <x14:cfRule type="cellIs" priority="24" operator="equal" id="{88C79D3D-BA54-4078-BD9E-2F9BC3DEFB72}">
             <xm:f>Słowniki!$C$2</xm:f>
             <x14:dxf>
               <font>
@@ -1427,7 +2857,7 @@
           <xm:sqref>G6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="9" operator="equal" id="{25F6B858-9AB9-4AE1-96C0-7EFEEB5DF4E4}">
+          <x14:cfRule type="cellIs" priority="21" operator="equal" id="{25F6B858-9AB9-4AE1-96C0-7EFEEB5DF4E4}">
             <xm:f>Słowniki!$C$3</xm:f>
             <x14:dxf>
               <font>
@@ -1440,7 +2870,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="10" operator="equal" id="{4E0E54DB-5892-43A5-B3EC-4025261B3444}">
+          <x14:cfRule type="cellIs" priority="22" operator="equal" id="{4E0E54DB-5892-43A5-B3EC-4025261B3444}">
             <xm:f>Słowniki!$C$2</xm:f>
             <x14:dxf>
               <font>
@@ -1456,7 +2886,7 @@
           <xm:sqref>G7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{CAAA9040-EFE1-4B54-8E74-8374721AC878}">
+          <x14:cfRule type="cellIs" priority="19" operator="equal" id="{CAAA9040-EFE1-4B54-8E74-8374721AC878}">
             <xm:f>Słowniki!$C$3</xm:f>
             <x14:dxf>
               <font>
@@ -1469,7 +2899,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{EFFF1C18-87DB-477C-8896-15090F84D0AA}">
+          <x14:cfRule type="cellIs" priority="20" operator="equal" id="{EFFF1C18-87DB-477C-8896-15090F84D0AA}">
             <xm:f>Słowniki!$C$2</xm:f>
             <x14:dxf>
               <font>
@@ -1485,7 +2915,7 @@
           <xm:sqref>G8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{AB2F79FB-2C5B-43FD-BE0B-873AC577B3BD}">
+          <x14:cfRule type="cellIs" priority="17" operator="equal" id="{AB2F79FB-2C5B-43FD-BE0B-873AC577B3BD}">
             <xm:f>Słowniki!$C$3</xm:f>
             <x14:dxf>
               <font>
@@ -1498,7 +2928,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{87990C9A-F18A-49D3-BF7E-D1FEFE654FDE}">
+          <x14:cfRule type="cellIs" priority="18" operator="equal" id="{87990C9A-F18A-49D3-BF7E-D1FEFE654FDE}">
             <xm:f>Słowniki!$C$2</xm:f>
             <x14:dxf>
               <font>
@@ -1514,7 +2944,7 @@
           <xm:sqref>G9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{08A98F56-2F89-40C1-ADA6-04BBFE89E413}">
+          <x14:cfRule type="cellIs" priority="15" operator="equal" id="{08A98F56-2F89-40C1-ADA6-04BBFE89E413}">
             <xm:f>Słowniki!$C$3</xm:f>
             <x14:dxf>
               <font>
@@ -1527,7 +2957,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{F6E770A7-2756-4A51-AB4C-268CC825E4D8}">
+          <x14:cfRule type="cellIs" priority="16" operator="equal" id="{F6E770A7-2756-4A51-AB4C-268CC825E4D8}">
             <xm:f>Słowniki!$C$2</xm:f>
             <x14:dxf>
               <font>
@@ -1540,7 +2970,181 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G10</xm:sqref>
+          <xm:sqref>G10 G12 G14 G16</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="9" operator="equal" id="{77DEB003-6562-4801-AA91-1AC27521B267}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="10" operator="equal" id="{BA6F90F8-25CC-4B46-A7A2-A04A102D998B}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="11" operator="equal" id="{245B49CA-9E03-4757-A344-5076A82AABD3}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="12" operator="equal" id="{0406A1DB-9FDB-4ADF-9CA4-8C41571A57C6}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G17 G19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{DED925FA-E058-4401-B0F1-C7E776613E1B}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{9F153EAE-076D-453C-8FB6-D283C4DFD416}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G21</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{C2FFCD20-5EF3-4676-8374-9413191528B7}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{0387969D-5BB3-4315-B1DD-BDBB155E7E4D}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G20 G22</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{51A0A744-3FB5-4B11-AD01-DD6B79A88C85}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{F64964BA-C24F-428A-9873-FDB89BF4A1C6}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{430EAEC9-C455-4D2A-A95D-FE0708B8DA28}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{9434112F-9DB0-4B57-A70A-D994ABD4520B}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G23 G25</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1550,13 +3154,13 @@
           <x14:formula1>
             <xm:f>Słowniki!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F4:F11</xm:sqref>
+          <xm:sqref>F4:F24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Słowniki!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G4:G11</xm:sqref>
+          <xm:sqref>G4:G25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1566,10 +3170,577 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="35.140625" customWidth="1"/>
+    <col min="3" max="3" width="69.5703125" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="2:7" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="B3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="7">
+        <v>5</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="13">
+        <v>3</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="99" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="7">
+        <v>3</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="7">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="7">
+        <v>3</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="7">
+        <v>5</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18">
+        <f>SUM(E5:E16)</f>
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="13" operator="equal" id="{7E363E78-2D8E-457E-9DFB-764213E8AAF6}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="14" operator="equal" id="{1B19C48B-5ADC-40A6-9BE4-0D55C0576CC8}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G5 G7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="15" operator="equal" id="{3DD390AE-4D8E-48B6-A451-3255C07000D0}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="16" operator="equal" id="{7D65F54D-4C3C-4526-A865-5DDC6E00B22D}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G6 G8</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="9" operator="equal" id="{8D84FDB5-C357-4E9A-8D77-513ACA9E1216}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="10" operator="equal" id="{5B23D1B7-1457-4F9F-A994-4CE05E95C7DF}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="11" operator="equal" id="{8574DB48-AC06-4ED6-BE05-C5812B157C26}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="12" operator="equal" id="{A2E6E152-FFDF-4D7C-AB8D-38564DDBF990}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G9 G11</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{5A4B8413-8431-45B8-B6F8-C0E847EA3846}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{6DDFB6B8-AF33-45D2-96C8-E27E74194CB6}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{F9B370F9-85AD-4968-B78D-22C2F80FB33C}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{C763ECDD-7A7D-491C-9867-225662F1E8E0}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G12 G14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{F4CEDFAA-8DD4-4946-A667-BF991852AD6B}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{14833D7A-45CF-45A3-8D27-34748039E35F}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G16</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{AB06B42E-B80B-45D0-BC76-7B5252FCC237}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{D87119E1-2AE1-41D8-9754-AE74F1693284}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G15</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Słowniki!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G5:G16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Słowniki!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>F5:F16</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G13"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1584,20 +3755,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="2:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -1758,7 +3929,7 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D13" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="9">
         <f>SUM(E4:E11)</f>
@@ -2022,12 +4193,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,7 +4227,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -2065,37 +4236,37 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" t="s">
         <v>43</v>
-      </c>
-      <c r="F7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E8" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dodano dzialajaca wersje produktu
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Damian\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\IPP30 Projects\SmartShop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pomysły" sheetId="2" r:id="rId1"/>
     <sheet name="Backlog" sheetId="5" r:id="rId2"/>
-    <sheet name="Sprint 1" sheetId="3" r:id="rId3"/>
-    <sheet name="Słowniki" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint 2" sheetId="6" r:id="rId3"/>
+    <sheet name="Sprint 1" sheetId="3" r:id="rId4"/>
+    <sheet name="Słowniki" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="88">
   <si>
     <t>Story</t>
   </si>
@@ -134,9 +135,6 @@
   </si>
   <si>
     <t>Niezrealizowane</t>
-  </si>
-  <si>
-    <t>#2</t>
   </si>
   <si>
     <t>#3</t>
@@ -193,12 +191,177 @@
   <si>
     <t>Wklej specjalnie -&gt; Zachowaj szerokości kolumn źródłowych</t>
   </si>
+  <si>
+    <t>Konto na smarterasp.net</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć utworzone konto na smartertasp.net abym mógł hostować tam webservice.</t>
+  </si>
+  <si>
+    <t>Utworzenie webservicu</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć utworzony webservice abym móg komunikować się z nim z aplikacji klienckiej</t>
+  </si>
+  <si>
+    <t>Upload webservicu na smartertasp.net</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć wrzucony webservice na smarterasp.net abym mógł komunikować się z nim zdalnie z aplikacji klienckiej</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć zaprojektowany i utworzony mock głównego widoku aplikacji klienckiej abym mógł zaimplementować do niego logike i podpiąć usługi</t>
+  </si>
+  <si>
+    <t>#2   06.04 - 27.04</t>
+  </si>
+  <si>
+    <t>Mock głównego widoku aplikacji klienckiej</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć utworzone modele danych odpowiadające tabelą w bazie danych, abym mógł korzystać z nich w aplikacji</t>
+  </si>
+  <si>
+    <t>klasy modeli dla tabel z bazy danych w projekcie SmartShopWpf, projekt się kompiluje</t>
+  </si>
+  <si>
+    <t>prawidłowo utworzone konto na smarterasp.net, przekazanie członkom zespołu informacji o danych do logowania</t>
+  </si>
+  <si>
+    <t>możliwość wykonania metod HTTP dla każdej z tabeli i uzyskanie prawidłowej odpowiedzi, projekt się kompiluje</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> prawidłowo zuploadowany webservice na smarterasp.net, możliwość wykonania metod HTTP dla każdej z tabeli i uzyskanie prawidłowej odpowiedzi</t>
+  </si>
+  <si>
+    <t>mock który jest dopasowany graficznie (kolory, czcionki itp) do mocka widoku logowania, podoba się wszystkim! i jest przygotowany do implementacji logiki zawartej w specyfikacji. Projekt się kompiluje.</t>
+  </si>
+  <si>
+    <t>Modele danych WPF</t>
+  </si>
+  <si>
+    <t>Zabezpieczenie brancha develop</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć zmodyfikowane ustawienia brancha develop, aby konieczne było wykonanie review przed commitem/mergem</t>
+  </si>
+  <si>
+    <t>zablokowana możliwość commitowania/mergowania do brancha develop, bez wcześniejszego wykonania rewiew</t>
+  </si>
+  <si>
+    <t>Mock widoku logowania</t>
+  </si>
+  <si>
+    <t>Jako developer chce mieć zaprojektowany i utworzony mock widoku logowania do aplikacji, abym mógł podpiąć do niego logikę i usługi weryfikujące poprawność wpisywanych danych logujących do systemu</t>
+  </si>
+  <si>
+    <t>mock który jest dopasowany graficznie (kolory, czcionki itp) do mocka widoku głównego, podoba się wszystkim! i jest przygotowany do implementacji logiki logowania. Projekt się kompiluje.</t>
+  </si>
+  <si>
+    <t>Modele danych WebApp</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć utworzone modele danych odpowiadające tabelą w bazie danych, abym mógł korzystać z nich w kontrolerach</t>
+  </si>
+  <si>
+    <t>klasy modeli dla tabel z bazy danych w projekcie SmartShopWebApp, projekt się kompiluje</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć zmodyfikowaną bazę danych, abym mógł przechowywać w niej informacje na temat kategorii danego produktu</t>
+  </si>
+  <si>
+    <t>Kategoria produktu w bazie danych</t>
+  </si>
+  <si>
+    <t>możliwość przechowywania informacji o kategorii produktu w bazie danych</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć zmodyfikowaną bazę danych, abym mógł przechowywać w niej zdjęcie danego produktu</t>
+  </si>
+  <si>
+    <t>pole w bazie danych przechowujące zdjęcie produktu</t>
+  </si>
+  <si>
+    <t>Zdjęcie produktu w bazie danych</t>
+  </si>
+  <si>
+    <t>Przykładowe produkty w bazie danych</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć dodane przykładowe produkty do bazy danych abym mógł je wykorzystywać w aplikacji</t>
+  </si>
+  <si>
+    <t>co najmniej 100 produktów w bazie danych z uzupełnionymi wszystkimi polami</t>
+  </si>
+  <si>
+    <t>Przygotowanie zdjęć produktów</t>
+  </si>
+  <si>
+    <t>Jako developer chcę mieć przygotowane zdjęcia dla produktów abym mógł je dodać do rekordów w bazie danych i wyświetlać je w aplikacji klienckiej</t>
+  </si>
+  <si>
+    <t>minimum 100 zdjęć, stosunkowo małych, o jednakowych wymiarach</t>
+  </si>
+  <si>
+    <t>Przejście pomiędzy widokami</t>
+  </si>
+  <si>
+    <t>Jako developer chce mieć zaimplementowane połączenie pomiędzy widokami logowania i głównym tak aby po zalogowaniu uruchamiał się widok główny aplikacji</t>
+  </si>
+  <si>
+    <t>przejście do widoku głównego, po naciśnięciu odpowiedniego przycisku w widoku logowania, przekazania danych o zalogowanym użytkowniku pomiędzy widokami</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Czas realizacji: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>06.04 - 27.04</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Suma </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>SP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,6 +456,13 @@
       <charset val="238"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -341,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -362,8 +532,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -371,423 +556,26 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="178">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="138">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2173,8 +1961,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="177"/>
-      <tableStyleElement type="headerRow" dxfId="176"/>
+      <tableStyleElement type="wholeTable" dxfId="137"/>
+      <tableStyleElement type="headerRow" dxfId="136"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -2453,7 +2241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -2464,7 +2252,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2474,10 +2262,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G11"/>
+  <dimension ref="B2:G25"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F11"/>
+    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2491,32 +2279,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2537,7 +2325,7 @@
         <v>31</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -2557,7 +2345,7 @@
         <v>31</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -2577,7 +2365,7 @@
         <v>31</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="75" x14ac:dyDescent="0.25">
@@ -2597,7 +2385,7 @@
         <v>31</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -2617,7 +2405,7 @@
         <v>31</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -2637,7 +2425,7 @@
         <v>31</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -2657,7 +2445,7 @@
         <v>31</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -2677,19 +2465,283 @@
         <v>31</v>
       </c>
       <c r="G11" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="7">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>34</v>
       </c>
+    </row>
+    <row r="13" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B13" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="7">
+        <v>5</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="7">
+        <v>1</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="13">
+        <v>3</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="7">
+        <v>1</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="7">
+        <v>3</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="7">
+        <v>1</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="7">
+        <v>3</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="7">
+        <v>5</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="7">
+        <v>1</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{35DA5DFD-158A-4A96-AFD3-16E6826D71F1}">
+          <x14:cfRule type="cellIs" priority="13" operator="equal" id="{35DA5DFD-158A-4A96-AFD3-16E6826D71F1}">
             <xm:f>Słowniki!$C$3</xm:f>
             <x14:dxf>
               <font>
@@ -2702,7 +2754,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{0EF4BF86-951E-4041-96BC-970E20B0F305}">
+          <x14:cfRule type="cellIs" priority="14" operator="equal" id="{0EF4BF86-951E-4041-96BC-970E20B0F305}">
             <xm:f>Słowniki!$C$2</xm:f>
             <x14:dxf>
               <font>
@@ -2715,10 +2767,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G11</xm:sqref>
+          <xm:sqref>G11 G13 G15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="15" operator="equal" id="{8CC48237-1EF7-42C0-8632-8CF6FA73EAAC}">
+          <x14:cfRule type="cellIs" priority="27" operator="equal" id="{8CC48237-1EF7-42C0-8632-8CF6FA73EAAC}">
             <xm:f>Słowniki!$C$3</xm:f>
             <x14:dxf>
               <font>
@@ -2731,7 +2783,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="16" operator="equal" id="{D4C76A03-45DE-4A75-9EB4-91E96096B768}">
+          <x14:cfRule type="cellIs" priority="28" operator="equal" id="{D4C76A03-45DE-4A75-9EB4-91E96096B768}">
             <xm:f>Słowniki!$C$2</xm:f>
             <x14:dxf>
               <font>
@@ -2747,7 +2799,7 @@
           <xm:sqref>G4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="13" operator="equal" id="{20C769E0-576E-4A5B-833F-BD175DCC8383}">
+          <x14:cfRule type="cellIs" priority="25" operator="equal" id="{20C769E0-576E-4A5B-833F-BD175DCC8383}">
             <xm:f>Słowniki!$C$3</xm:f>
             <x14:dxf>
               <font>
@@ -2760,7 +2812,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="14" operator="equal" id="{104971B7-D297-494A-AD75-9138BA5AC24C}">
+          <x14:cfRule type="cellIs" priority="26" operator="equal" id="{104971B7-D297-494A-AD75-9138BA5AC24C}">
             <xm:f>Słowniki!$C$2</xm:f>
             <x14:dxf>
               <font>
@@ -2776,7 +2828,7 @@
           <xm:sqref>G5</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="11" operator="equal" id="{F781F71C-1B94-4299-AC7C-06FA0D1D02FD}">
+          <x14:cfRule type="cellIs" priority="23" operator="equal" id="{F781F71C-1B94-4299-AC7C-06FA0D1D02FD}">
             <xm:f>Słowniki!$C$3</xm:f>
             <x14:dxf>
               <font>
@@ -2789,7 +2841,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="12" operator="equal" id="{88C79D3D-BA54-4078-BD9E-2F9BC3DEFB72}">
+          <x14:cfRule type="cellIs" priority="24" operator="equal" id="{88C79D3D-BA54-4078-BD9E-2F9BC3DEFB72}">
             <xm:f>Słowniki!$C$2</xm:f>
             <x14:dxf>
               <font>
@@ -2805,7 +2857,7 @@
           <xm:sqref>G6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="9" operator="equal" id="{25F6B858-9AB9-4AE1-96C0-7EFEEB5DF4E4}">
+          <x14:cfRule type="cellIs" priority="21" operator="equal" id="{25F6B858-9AB9-4AE1-96C0-7EFEEB5DF4E4}">
             <xm:f>Słowniki!$C$3</xm:f>
             <x14:dxf>
               <font>
@@ -2818,7 +2870,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="10" operator="equal" id="{4E0E54DB-5892-43A5-B3EC-4025261B3444}">
+          <x14:cfRule type="cellIs" priority="22" operator="equal" id="{4E0E54DB-5892-43A5-B3EC-4025261B3444}">
             <xm:f>Słowniki!$C$2</xm:f>
             <x14:dxf>
               <font>
@@ -2834,7 +2886,7 @@
           <xm:sqref>G7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{CAAA9040-EFE1-4B54-8E74-8374721AC878}">
+          <x14:cfRule type="cellIs" priority="19" operator="equal" id="{CAAA9040-EFE1-4B54-8E74-8374721AC878}">
             <xm:f>Słowniki!$C$3</xm:f>
             <x14:dxf>
               <font>
@@ -2847,7 +2899,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{EFFF1C18-87DB-477C-8896-15090F84D0AA}">
+          <x14:cfRule type="cellIs" priority="20" operator="equal" id="{EFFF1C18-87DB-477C-8896-15090F84D0AA}">
             <xm:f>Słowniki!$C$2</xm:f>
             <x14:dxf>
               <font>
@@ -2863,7 +2915,7 @@
           <xm:sqref>G8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{AB2F79FB-2C5B-43FD-BE0B-873AC577B3BD}">
+          <x14:cfRule type="cellIs" priority="17" operator="equal" id="{AB2F79FB-2C5B-43FD-BE0B-873AC577B3BD}">
             <xm:f>Słowniki!$C$3</xm:f>
             <x14:dxf>
               <font>
@@ -2876,7 +2928,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{87990C9A-F18A-49D3-BF7E-D1FEFE654FDE}">
+          <x14:cfRule type="cellIs" priority="18" operator="equal" id="{87990C9A-F18A-49D3-BF7E-D1FEFE654FDE}">
             <xm:f>Słowniki!$C$2</xm:f>
             <x14:dxf>
               <font>
@@ -2892,7 +2944,7 @@
           <xm:sqref>G9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{08A98F56-2F89-40C1-ADA6-04BBFE89E413}">
+          <x14:cfRule type="cellIs" priority="15" operator="equal" id="{08A98F56-2F89-40C1-ADA6-04BBFE89E413}">
             <xm:f>Słowniki!$C$3</xm:f>
             <x14:dxf>
               <font>
@@ -2905,7 +2957,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{F6E770A7-2756-4A51-AB4C-268CC825E4D8}">
+          <x14:cfRule type="cellIs" priority="16" operator="equal" id="{F6E770A7-2756-4A51-AB4C-268CC825E4D8}">
             <xm:f>Słowniki!$C$2</xm:f>
             <x14:dxf>
               <font>
@@ -2918,7 +2970,181 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G10</xm:sqref>
+          <xm:sqref>G10 G12 G14 G16</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="9" operator="equal" id="{77DEB003-6562-4801-AA91-1AC27521B267}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="10" operator="equal" id="{BA6F90F8-25CC-4B46-A7A2-A04A102D998B}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="11" operator="equal" id="{245B49CA-9E03-4757-A344-5076A82AABD3}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="12" operator="equal" id="{0406A1DB-9FDB-4ADF-9CA4-8C41571A57C6}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G17 G19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{DED925FA-E058-4401-B0F1-C7E776613E1B}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{9F153EAE-076D-453C-8FB6-D283C4DFD416}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G21</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{C2FFCD20-5EF3-4676-8374-9413191528B7}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{0387969D-5BB3-4315-B1DD-BDBB155E7E4D}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G20 G22</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{51A0A744-3FB5-4B11-AD01-DD6B79A88C85}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{F64964BA-C24F-428A-9873-FDB89BF4A1C6}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{430EAEC9-C455-4D2A-A95D-FE0708B8DA28}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{9434112F-9DB0-4B57-A70A-D994ABD4520B}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G23 G25</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2928,13 +3154,13 @@
           <x14:formula1>
             <xm:f>Słowniki!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F4:F11</xm:sqref>
+          <xm:sqref>F4:F24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Słowniki!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G4:G11</xm:sqref>
+          <xm:sqref>G4:G25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2944,10 +3170,577 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="35.140625" customWidth="1"/>
+    <col min="3" max="3" width="69.5703125" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="2:7" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="B3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="7">
+        <v>5</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="13">
+        <v>3</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="99" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="7">
+        <v>3</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="7">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="7">
+        <v>3</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="7">
+        <v>5</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18">
+        <f>SUM(E5:E16)</f>
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="13" operator="equal" id="{7E363E78-2D8E-457E-9DFB-764213E8AAF6}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="14" operator="equal" id="{1B19C48B-5ADC-40A6-9BE4-0D55C0576CC8}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G5 G7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="15" operator="equal" id="{3DD390AE-4D8E-48B6-A451-3255C07000D0}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="16" operator="equal" id="{7D65F54D-4C3C-4526-A865-5DDC6E00B22D}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G6 G8</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="9" operator="equal" id="{8D84FDB5-C357-4E9A-8D77-513ACA9E1216}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="10" operator="equal" id="{5B23D1B7-1457-4F9F-A994-4CE05E95C7DF}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="11" operator="equal" id="{8574DB48-AC06-4ED6-BE05-C5812B157C26}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="12" operator="equal" id="{A2E6E152-FFDF-4D7C-AB8D-38564DDBF990}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G9 G11</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{5A4B8413-8431-45B8-B6F8-C0E847EA3846}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{6DDFB6B8-AF33-45D2-96C8-E27E74194CB6}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G13</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{F9B370F9-85AD-4968-B78D-22C2F80FB33C}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{C763ECDD-7A7D-491C-9867-225662F1E8E0}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G12 G14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{F4CEDFAA-8DD4-4946-A667-BF991852AD6B}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{14833D7A-45CF-45A3-8D27-34748039E35F}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G16</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{AB06B42E-B80B-45D0-BC76-7B5252FCC237}">
+            <xm:f>Słowniki!$C$3</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{D87119E1-2AE1-41D8-9754-AE74F1693284}">
+            <xm:f>Słowniki!$C$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G15</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Słowniki!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G5:G16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Słowniki!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>F5:F16</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G13"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2962,39 +3755,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="2:7" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3135,8 +3928,8 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="15" t="s">
-        <v>41</v>
+      <c r="D13" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="E13" s="9">
         <f>SUM(E4:E11)</f>
@@ -3400,12 +4193,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3434,7 +4227,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -3443,37 +4236,37 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" t="s">
         <v>43</v>
       </c>
-      <c r="F7" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="12" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="16" t="s">
+      <c r="F8" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>